<commit_message>
Added shipping, discount and due date
</commit_message>
<xml_diff>
--- a/invoice_details.xlsx
+++ b/invoice_details.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Learning\Invoice Generator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44317488-C614-436A-96D9-9071188FF6CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7207D47-39E1-4B57-8DC1-AB624583A1AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="138">
   <si>
     <t>Client Name</t>
   </si>
@@ -303,9 +303,6 @@
     <t>Magical Motorbike Accessory</t>
   </si>
   <si>
-    <t>Hogsmeade Garage, Scotland</t>
-  </si>
-  <si>
     <t>INV015</t>
   </si>
   <si>
@@ -435,19 +432,13 @@
     <t>Elder Wand Replica</t>
   </si>
   <si>
-    <t>Forbidden Forest, Hogwarts Grounds, Scotland</t>
-  </si>
-  <si>
     <t>Parseltongue Dictionary</t>
   </si>
   <si>
-    <t>Little Hangleton Graveyard, England</t>
-  </si>
-  <si>
     <t>Nagini Care Kit</t>
   </si>
   <si>
-    <t>Dark Forest Cavern, Albania</t>
+    <t>Shipping Charges</t>
   </si>
 </sst>
 </file>
@@ -796,10 +787,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K38"/>
+  <dimension ref="A1:L38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="H43" sqref="H43"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="K40" sqref="K40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -815,7 +806,7 @@
     <col min="10" max="11" width="35.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>42</v>
       </c>
@@ -849,8 +840,11 @@
       <c r="K1" s="2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L1" s="2" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>10</v>
       </c>
@@ -884,8 +878,11 @@
       <c r="K2" s="3" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L2">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>10</v>
       </c>
@@ -919,8 +916,11 @@
       <c r="K3" s="3" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L3">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>18</v>
       </c>
@@ -954,8 +954,11 @@
       <c r="K4" s="3" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>18</v>
       </c>
@@ -989,8 +992,11 @@
       <c r="K5" s="3" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L5">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>23</v>
       </c>
@@ -1024,8 +1030,11 @@
       <c r="K6" s="3" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L6">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>27</v>
       </c>
@@ -1059,8 +1068,11 @@
       <c r="K7" s="3" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L7">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
         <v>32</v>
       </c>
@@ -1094,8 +1106,11 @@
       <c r="K8" s="3" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L8">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
         <v>32</v>
       </c>
@@ -1129,8 +1144,11 @@
       <c r="K9" s="3" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L9">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
         <v>32</v>
       </c>
@@ -1164,8 +1182,11 @@
       <c r="K10" s="3" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="11" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="L10">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
         <v>32</v>
       </c>
@@ -1199,8 +1220,11 @@
       <c r="K11" s="3" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L11">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
         <v>37</v>
       </c>
@@ -1234,8 +1258,11 @@
       <c r="K12" s="3" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L12">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
         <v>37</v>
       </c>
@@ -1269,8 +1296,11 @@
       <c r="K13" s="3" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="14" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="L13">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
         <v>39</v>
       </c>
@@ -1304,8 +1334,11 @@
       <c r="K14" s="3" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L14">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
         <v>40</v>
       </c>
@@ -1339,8 +1372,11 @@
       <c r="K15" s="3" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L15">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
         <v>40</v>
       </c>
@@ -1374,8 +1410,11 @@
       <c r="K16" s="3" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L16">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
         <v>40</v>
       </c>
@@ -1409,8 +1448,11 @@
       <c r="K17" s="3" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="18" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="L17">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
         <v>41</v>
       </c>
@@ -1444,8 +1486,11 @@
       <c r="K18" s="3" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="19" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="L18">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="s">
         <v>64</v>
       </c>
@@ -1479,8 +1524,11 @@
       <c r="K19" s="3" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="20" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="L19">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A20" s="3" t="s">
         <v>64</v>
       </c>
@@ -1514,8 +1562,11 @@
       <c r="K20" s="3" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="21" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="L20">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A21" s="3" t="s">
         <v>71</v>
       </c>
@@ -1549,8 +1600,11 @@
       <c r="K21" s="3" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A22" s="3" t="s">
         <v>71</v>
       </c>
@@ -1584,8 +1638,11 @@
       <c r="K22" s="3" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="23" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="L22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A23" s="3" t="s">
         <v>78</v>
       </c>
@@ -1619,8 +1676,11 @@
       <c r="K23" s="3" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="24" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="L23">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A24" s="3" t="s">
         <v>78</v>
       </c>
@@ -1654,8 +1714,11 @@
       <c r="K24" s="3" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="25" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="L24">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A25" s="3" t="s">
         <v>86</v>
       </c>
@@ -1689,8 +1752,11 @@
       <c r="K25" s="3" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="26" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="L25">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A26" s="3" t="s">
         <v>86</v>
       </c>
@@ -1722,18 +1788,21 @@
         <v>15</v>
       </c>
       <c r="K26" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="L26">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A27" s="3" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="27" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A27" s="3" t="s">
+      <c r="B27" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="B27" s="3" t="s">
+      <c r="C27" s="4" t="s">
         <v>94</v>
-      </c>
-      <c r="C27" s="4" t="s">
-        <v>95</v>
       </c>
       <c r="D27" s="5">
         <v>45787</v>
@@ -1742,7 +1811,7 @@
         <v>45818</v>
       </c>
       <c r="F27" s="3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G27" s="3">
         <v>1</v>
@@ -1751,24 +1820,27 @@
         <v>1000</v>
       </c>
       <c r="I27" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="J27" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="J27" s="3" t="s">
+      <c r="K27" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="K27" s="3" t="s">
+      <c r="L27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A28" s="3" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="28" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A28" s="3" t="s">
+      <c r="B28" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="B28" s="3" t="s">
+      <c r="C28" s="4" t="s">
         <v>101</v>
-      </c>
-      <c r="C28" s="4" t="s">
-        <v>102</v>
       </c>
       <c r="D28" s="5">
         <v>45788</v>
@@ -1777,7 +1849,7 @@
         <v>45819</v>
       </c>
       <c r="F28" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="G28" s="3">
         <v>7</v>
@@ -1789,21 +1861,24 @@
         <v>14</v>
       </c>
       <c r="J28" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="K28" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="K28" s="3" t="s">
+      <c r="L28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A29" s="3" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="29" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A29" s="3" t="s">
+      <c r="B29" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="B29" s="3" t="s">
+      <c r="C29" s="4" t="s">
         <v>107</v>
-      </c>
-      <c r="C29" s="4" t="s">
-        <v>108</v>
       </c>
       <c r="D29" s="5">
         <v>45789</v>
@@ -1812,7 +1887,7 @@
         <v>45820</v>
       </c>
       <c r="F29" s="3" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="G29" s="3">
         <v>1</v>
@@ -1821,24 +1896,27 @@
         <v>500</v>
       </c>
       <c r="I29" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="J29" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="J29" s="3" t="s">
+      <c r="K29" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="K29" s="3" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="30" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="L29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A30" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="B30" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="B30" s="3" t="s">
+      <c r="C30" s="4" t="s">
         <v>107</v>
-      </c>
-      <c r="C30" s="4" t="s">
-        <v>108</v>
       </c>
       <c r="D30" s="5">
         <v>45789</v>
@@ -1847,7 +1925,7 @@
         <v>45820</v>
       </c>
       <c r="F30" s="3" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="G30" s="3">
         <v>5</v>
@@ -1856,24 +1934,27 @@
         <v>50</v>
       </c>
       <c r="I30" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="J30" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="J30" s="3" t="s">
+      <c r="K30" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="K30" s="3" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A31" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="B31" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="B31" s="3" t="s">
+      <c r="C31" s="4" t="s">
         <v>115</v>
-      </c>
-      <c r="C31" s="4" t="s">
-        <v>116</v>
       </c>
       <c r="D31" s="5">
         <v>45790</v>
@@ -1882,7 +1963,7 @@
         <v>45821</v>
       </c>
       <c r="F31" s="3" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="G31" s="3">
         <v>10</v>
@@ -1894,21 +1975,24 @@
         <v>17</v>
       </c>
       <c r="J31" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="K31" s="3" t="s">
         <v>118</v>
       </c>
-      <c r="K31" s="3" t="s">
+      <c r="L31">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A32" s="3" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="32" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A32" s="3" t="s">
+      <c r="B32" s="3" t="s">
         <v>120</v>
       </c>
-      <c r="B32" s="3" t="s">
+      <c r="C32" s="4" t="s">
         <v>121</v>
-      </c>
-      <c r="C32" s="4" t="s">
-        <v>122</v>
       </c>
       <c r="D32" s="5">
         <v>45790</v>
@@ -1917,7 +2001,7 @@
         <v>45821</v>
       </c>
       <c r="F32" s="3" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="G32" s="3">
         <v>6</v>
@@ -1926,24 +2010,27 @@
         <v>60</v>
       </c>
       <c r="I32" s="3" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="J32" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="K32" s="3" t="s">
         <v>124</v>
       </c>
-      <c r="K32" s="3" t="s">
+      <c r="L32">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A33" s="3" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A33" s="3" t="s">
+      <c r="B33" s="3" t="s">
         <v>126</v>
       </c>
-      <c r="B33" s="3" t="s">
+      <c r="C33" s="4" t="s">
         <v>127</v>
-      </c>
-      <c r="C33" s="4" t="s">
-        <v>128</v>
       </c>
       <c r="D33" s="5">
         <v>45791</v>
@@ -1952,7 +2039,7 @@
         <v>45822</v>
       </c>
       <c r="F33" s="3" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="G33" s="3">
         <v>1</v>
@@ -1961,24 +2048,27 @@
         <v>1000</v>
       </c>
       <c r="I33" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="J33" s="3" t="s">
         <v>130</v>
       </c>
-      <c r="J33" s="3" t="s">
+      <c r="K33" s="3" t="s">
         <v>131</v>
       </c>
-      <c r="K33" s="3" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L33">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A34" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="B34" s="3" t="s">
         <v>126</v>
       </c>
-      <c r="B34" s="3" t="s">
+      <c r="C34" s="4" t="s">
         <v>127</v>
-      </c>
-      <c r="C34" s="4" t="s">
-        <v>128</v>
       </c>
       <c r="D34" s="5">
         <v>45791</v>
@@ -1987,7 +2077,7 @@
         <v>45822</v>
       </c>
       <c r="F34" s="3" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="G34" s="3">
         <v>2</v>
@@ -1996,24 +2086,27 @@
         <v>800</v>
       </c>
       <c r="I34" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="J34" s="3" t="s">
         <v>130</v>
       </c>
-      <c r="J34" s="3" t="s">
+      <c r="K34" s="3" t="s">
         <v>131</v>
       </c>
-      <c r="K34" s="3" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="35" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="L34">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A35" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="B35" s="3" t="s">
         <v>126</v>
       </c>
-      <c r="B35" s="3" t="s">
+      <c r="C35" s="4" t="s">
         <v>127</v>
-      </c>
-      <c r="C35" s="4" t="s">
-        <v>128</v>
       </c>
       <c r="D35" s="5">
         <v>45791</v>
@@ -2022,7 +2115,7 @@
         <v>45822</v>
       </c>
       <c r="F35" s="3" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="G35" s="3">
         <v>5</v>
@@ -2031,24 +2124,27 @@
         <v>300</v>
       </c>
       <c r="I35" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="J35" s="3" t="s">
         <v>130</v>
       </c>
-      <c r="J35" s="3" t="s">
+      <c r="K35" s="3" t="s">
         <v>131</v>
       </c>
-      <c r="K35" s="3" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="36" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="L35">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A36" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="B36" s="3" t="s">
         <v>126</v>
       </c>
-      <c r="B36" s="3" t="s">
+      <c r="C36" s="4" t="s">
         <v>127</v>
-      </c>
-      <c r="C36" s="4" t="s">
-        <v>128</v>
       </c>
       <c r="D36" s="5">
         <v>45791</v>
@@ -2057,7 +2153,7 @@
         <v>45822</v>
       </c>
       <c r="F36" s="3" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="G36" s="3">
         <v>1</v>
@@ -2066,24 +2162,27 @@
         <v>1500</v>
       </c>
       <c r="I36" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="J36" s="3" t="s">
         <v>130</v>
       </c>
-      <c r="J36" s="3" t="s">
+      <c r="K36" s="3" t="s">
         <v>131</v>
       </c>
-      <c r="K36" s="3" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="37" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="L36">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A37" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="B37" s="3" t="s">
         <v>126</v>
       </c>
-      <c r="B37" s="3" t="s">
+      <c r="C37" s="4" t="s">
         <v>127</v>
-      </c>
-      <c r="C37" s="4" t="s">
-        <v>128</v>
       </c>
       <c r="D37" s="5">
         <v>45791</v>
@@ -2092,7 +2191,7 @@
         <v>45822</v>
       </c>
       <c r="F37" s="3" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="G37" s="3">
         <v>3</v>
@@ -2101,24 +2200,27 @@
         <v>120</v>
       </c>
       <c r="I37" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="J37" s="3" t="s">
         <v>130</v>
       </c>
-      <c r="J37" s="3" t="s">
+      <c r="K37" s="3" t="s">
         <v>131</v>
       </c>
-      <c r="K37" s="3" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L37">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A38" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="B38" s="3" t="s">
         <v>126</v>
       </c>
-      <c r="B38" s="3" t="s">
+      <c r="C38" s="4" t="s">
         <v>127</v>
-      </c>
-      <c r="C38" s="4" t="s">
-        <v>128</v>
       </c>
       <c r="D38" s="5">
         <v>45791</v>
@@ -2127,7 +2229,7 @@
         <v>45822</v>
       </c>
       <c r="F38" s="3" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="G38" s="3">
         <v>2</v>
@@ -2136,13 +2238,16 @@
         <v>250</v>
       </c>
       <c r="I38" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="J38" s="3" t="s">
         <v>130</v>
       </c>
-      <c r="J38" s="3" t="s">
+      <c r="K38" s="3" t="s">
         <v>131</v>
       </c>
-      <c r="K38" s="3" t="s">
-        <v>140</v>
+      <c r="L38">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>